<commit_message>
Update statistike nakon dodavanja novih stvari
</commit_message>
<xml_diff>
--- a/dokumentacija/broj_linija_postotak.xlsx
+++ b/dokumentacija/broj_linija_postotak.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibrisevic\Desktop\Faris\Fakultet\IV semestar\Web dizajn\ferrari_stranica\dokumentacija\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{30EC602C-2818-473D-9E09-3F93F6B79267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F5AA79-32D6-4406-9694-10745B28E8BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{42ECB29D-4F5C-454C-8EE2-6E2C2DD86F5F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>index.html</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t xml:space="preserve">Ukupno: </t>
+  </si>
+  <si>
+    <t>graphs.js</t>
   </si>
 </sst>
 </file>
@@ -104,7 +107,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -163,7 +166,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -481,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2EB1FF2-2B9F-44C3-8725-BA06A33CE680}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -618,7 +621,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -668,7 +671,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -676,65 +679,67 @@
         <v>173</v>
       </c>
       <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="1">
         <v>103</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
+      <c r="D18" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="2">
-        <f>SUM(B1:B18)</f>
-        <v>2844</v>
-      </c>
-      <c r="C19" s="2">
+      <c r="E18" s="2">
+        <f>SUM(B1:B19)</f>
+        <v>2878</v>
+      </c>
+      <c r="F18" s="2">
         <f>SUM(B1,B2,B3,B4,B5,B6,B7,B9,B12,B14,B16)</f>
-        <v>1108</v>
-      </c>
-      <c r="D19" s="2">
+        <v>1113</v>
+      </c>
+      <c r="G18" s="2">
         <f>SUM(B8,B10,B13,B17,B15)</f>
         <v>1522</v>
       </c>
-      <c r="E19" s="2">
-        <f>SUM(B11,B18)</f>
-        <v>214</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
+      <c r="H18" s="2">
+        <f>SUM(B11,B18,B19)</f>
+        <v>243</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="1">
+        <v>29</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="4">
-        <f>(C19/B19)*100</f>
-        <v>38.959212376933891</v>
-      </c>
-      <c r="D20" s="4">
-        <f>(D19/B19)*100</f>
-        <v>53.51617440225035</v>
-      </c>
-      <c r="E20" s="4">
-        <f>(E19/B19)*100</f>
-        <v>7.5246132208157528</v>
+      <c r="F19" s="4">
+        <f>(F18/E18)*100</f>
+        <v>38.6726893676164</v>
+      </c>
+      <c r="G19" s="4">
+        <f>(G18/E18)*100</f>
+        <v>52.883947185545523</v>
+      </c>
+      <c r="H19" s="4">
+        <f>(H18/E18)*100</f>
+        <v>8.4433634468380809</v>
       </c>
     </row>
   </sheetData>

</xml_diff>